<commit_message>
DTS-1 final login test
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tranp\Desktop\Study-software-testing-engineer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7712ED-4C73-4A8B-A752-3879B1F206ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3D018E-C76E-4001-99E0-F92921275B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Project Name</t>
   </si>
@@ -130,9 +130,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Ready</t>
-  </si>
-  <si>
     <t>Valid URL
 Test Data</t>
   </si>
@@ -187,16 +184,23 @@
   </si>
   <si>
     <t>An error occurred while processing your request. Please try again</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>31/5/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -238,9 +242,17 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
       <color rgb="FF1C1E21"/>
-      <name val="Inherit"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -411,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,10 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -465,6 +474,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -480,20 +498,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -518,6 +541,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -525,14 +555,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -753,21 +776,24 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="31.88671875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="31.21875" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13.2">
+    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13.2">
+    <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -783,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="13.2">
+    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -791,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13.2">
+    <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -799,21 +825,21 @@
         <v>45442</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="13.2">
+    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="13.2">
+    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="13.2">
+    <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -829,15 +855,15 @@
         <v>14</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -849,18 +875,18 @@
       <c r="M9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="39.6">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:14" ht="66" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -870,147 +896,185 @@
         <v>32</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="28"/>
+      <c r="K10" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="L10" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="12"/>
-    </row>
-    <row r="11" spans="1:14" ht="39.6">
-      <c r="A11" s="27"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="17" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:14" ht="26.4">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="31">
+        <v>45443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="17" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="1:14" ht="39.6">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="31">
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:14" ht="52.8">
-      <c r="A14" s="27"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="31">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" ht="73.8" customHeight="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="18"/>
+      <c r="M14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14" s="31">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1025,9 +1089,9 @@
       <c r="M15" s="10"/>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" ht="13.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+    <row r="16" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="12"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1041,7 +1105,7 @@
       <c r="M16" s="10"/>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="1:14" ht="13.2">
+    <row r="17" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="9"/>
       <c r="C17" s="12"/>
@@ -1057,7 +1121,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:14" ht="13.2">
+    <row r="18" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="12"/>
@@ -1073,7 +1137,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="1:14" ht="13.2">
+    <row r="19" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="8"/>
@@ -1089,7 +1153,7 @@
       <c r="M19" s="7"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" ht="13.2">
+    <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="8"/>
@@ -1105,7 +1169,7 @@
       <c r="M20" s="7"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" ht="13.2">
+    <row r="21" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="8"/>
@@ -1126,15 +1190,21 @@
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
   </mergeCells>
-  <conditionalFormatting sqref="L10">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="L10:L14">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -1162,7 +1232,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>